<commit_message>
Fixed a DocType ID
</commit_message>
<xml_diff>
--- a/Code Lists/TOOP CL Document types v1.xlsx
+++ b/Code Lists/TOOP CL Document types v1.xlsx
@@ -42,13 +42,13 @@
     <t>Deprecated since</t>
   </si>
   <si>
-    <t>urn:eu:toop:ns:dataexchange-1p10::Request##urn:eu.toop.response.registeredorganization::1.10</t>
-  </si>
-  <si>
     <t>urn:eu:toop:ns:dataexchange-1p10::Request##urn:eu.toop.request.registeredorganization::1.10</t>
   </si>
   <si>
     <t>Registered Organization</t>
+  </si>
+  <si>
+    <t>urn:eu:toop:ns:dataexchange-1p10::Response##urn:eu.toop.response.registeredorganization::1.10</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:D5"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -577,10 +577,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -590,12 +590,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="29">
       <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Micro adoptions for code generation
</commit_message>
<xml_diff>
--- a/Code Lists/TOOP CL Document types v1.xlsx
+++ b/Code Lists/TOOP CL Document types v1.xlsx
@@ -30,9 +30,6 @@
     <t>Common Name</t>
   </si>
   <si>
-    <t>PEPPOL Document Identifier</t>
-  </si>
-  <si>
     <t>Since</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>urn:eu:toop:ns:dataexchange-1p10::Response##urn:eu.toop.response.registeredorganization::1.10</t>
+  </si>
+  <si>
+    <t>TOOP Document Type Identifier</t>
   </si>
 </sst>
 </file>
@@ -114,28 +114,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,81 +535,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="6"/>
+    <col min="1" max="1" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6">
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="b">
+      <c r="D2" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="b">
+      <c r="D3" s="1" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E3"/>

</xml_diff>